<commit_message>
mise a jour BOM
j'ai ajouté les prix
</commit_message>
<xml_diff>
--- a/structure/BOM.xlsx
+++ b/structure/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loic-\Documents\projects\RecuH2O\structure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{153F5CA6-5F52-433D-B1A3-826FD388C968}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{659DC37A-DF69-4C18-89DA-EACF649FD29F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -891,6 +891,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -900,12 +906,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2156,11 +2156,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:4" ht="50.1" customHeight="1">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
     </row>
     <row r="7" spans="2:4" ht="18.75">
       <c r="B7" s="1" t="s">
@@ -2207,8 +2207,8 @@
   </sheetPr>
   <dimension ref="A1:IV36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="J26" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" customHeight="1"/>
@@ -2328,7 +2328,7 @@
       </c>
       <c r="C5" s="25">
         <f>E32</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="22"/>
       <c r="E5" s="16"/>
@@ -2352,7 +2352,7 @@
       </c>
       <c r="C6" s="26">
         <f>O32</f>
-        <v>5</v>
+        <v>140.49</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="16"/>
@@ -2452,7 +2452,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="35"/>
-      <c r="G9" s="78" t="s">
+      <c r="G9" s="74" t="s">
         <v>57</v>
       </c>
       <c r="H9" s="21"/>
@@ -2463,10 +2463,12 @@
       <c r="K9" s="21"/>
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
-      <c r="N9" s="37"/>
+      <c r="N9" s="37">
+        <v>22.8</v>
+      </c>
       <c r="O9" s="38">
         <f t="shared" ref="O9:O31" si="0">E9*N9</f>
-        <v>0</v>
+        <v>22.8</v>
       </c>
       <c r="P9" s="33"/>
       <c r="Q9" s="39" t="s">
@@ -2489,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="35"/>
-      <c r="G10" s="79" t="s">
+      <c r="G10" s="75" t="s">
         <v>59</v>
       </c>
       <c r="H10" s="41"/>
@@ -2528,7 +2530,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="35"/>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="75" t="s">
         <v>58</v>
       </c>
       <c r="H11" s="41"/>
@@ -2539,10 +2541,12 @@
       <c r="K11" s="41"/>
       <c r="L11" s="41"/>
       <c r="M11" s="41"/>
-      <c r="N11" s="37"/>
+      <c r="N11" s="37">
+        <v>7.37</v>
+      </c>
       <c r="O11" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.37</v>
       </c>
       <c r="P11" s="33"/>
       <c r="Q11" s="44" t="s">
@@ -2565,7 +2569,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="35"/>
-      <c r="G12" s="79" t="s">
+      <c r="G12" s="75" t="s">
         <v>60</v>
       </c>
       <c r="H12" s="41"/>
@@ -2576,10 +2580,12 @@
       <c r="K12" s="41"/>
       <c r="L12" s="41"/>
       <c r="M12" s="41"/>
-      <c r="N12" s="37"/>
+      <c r="N12" s="37">
+        <v>9.99</v>
+      </c>
       <c r="O12" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.99</v>
       </c>
       <c r="P12" s="33"/>
       <c r="Q12" s="45" t="s">
@@ -2602,7 +2608,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="35"/>
-      <c r="G13" s="79" t="s">
+      <c r="G13" s="75" t="s">
         <v>61</v>
       </c>
       <c r="H13" s="41"/>
@@ -2611,10 +2617,12 @@
       <c r="K13" s="41"/>
       <c r="L13" s="41"/>
       <c r="M13" s="41"/>
-      <c r="N13" s="37"/>
+      <c r="N13" s="37">
+        <v>22</v>
+      </c>
       <c r="O13" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="P13" s="47"/>
       <c r="Q13" s="48"/>
@@ -2635,7 +2643,7 @@
         <v>2</v>
       </c>
       <c r="F14" s="35"/>
-      <c r="G14" s="79" t="s">
+      <c r="G14" s="75" t="s">
         <v>62</v>
       </c>
       <c r="H14" s="41"/>
@@ -2644,10 +2652,12 @@
       <c r="K14" s="41"/>
       <c r="L14" s="41"/>
       <c r="M14" s="41"/>
-      <c r="N14" s="37"/>
+      <c r="N14" s="37">
+        <v>17.2</v>
+      </c>
       <c r="O14" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>34.4</v>
       </c>
       <c r="P14" s="47"/>
       <c r="Q14" s="19"/>
@@ -2668,7 +2678,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="35"/>
-      <c r="G15" s="79" t="s">
+      <c r="G15" s="75" t="s">
         <v>63</v>
       </c>
       <c r="H15" s="41"/>
@@ -2677,10 +2687,12 @@
       <c r="K15" s="41"/>
       <c r="L15" s="41"/>
       <c r="M15" s="41"/>
-      <c r="N15" s="37"/>
+      <c r="N15" s="37">
+        <v>15</v>
+      </c>
       <c r="O15" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="P15" s="47"/>
       <c r="Q15" s="19"/>
@@ -2701,7 +2713,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="35"/>
-      <c r="G16" s="78" t="s">
+      <c r="G16" s="74" t="s">
         <v>66</v>
       </c>
       <c r="H16" s="21"/>
@@ -2710,10 +2722,12 @@
       <c r="K16" s="21"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
-      <c r="N16" s="37"/>
+      <c r="N16" s="37">
+        <v>10.130000000000001</v>
+      </c>
       <c r="O16" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10.130000000000001</v>
       </c>
       <c r="P16" s="47"/>
       <c r="Q16" s="19"/>
@@ -2734,7 +2748,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="35"/>
-      <c r="G17" s="79" t="s">
+      <c r="G17" s="75" t="s">
         <v>67</v>
       </c>
       <c r="H17" s="41"/>
@@ -2743,10 +2757,12 @@
       <c r="K17" s="41"/>
       <c r="L17" s="41"/>
       <c r="M17" s="41"/>
-      <c r="N17" s="37"/>
+      <c r="N17" s="37">
+        <v>3.81</v>
+      </c>
       <c r="O17" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.81</v>
       </c>
       <c r="P17" s="47"/>
       <c r="Q17" s="19"/>
@@ -2764,10 +2780,10 @@
         <v>56</v>
       </c>
       <c r="E18" s="35">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F18" s="35"/>
-      <c r="G18" s="79" t="s">
+      <c r="G18" s="75" t="s">
         <v>68</v>
       </c>
       <c r="H18" s="41"/>
@@ -2776,10 +2792,12 @@
       <c r="K18" s="41"/>
       <c r="L18" s="41"/>
       <c r="M18" s="41"/>
-      <c r="N18" s="37"/>
+      <c r="N18" s="37">
+        <v>9.99</v>
+      </c>
       <c r="O18" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.99</v>
       </c>
       <c r="P18" s="47"/>
       <c r="Q18" s="19"/>
@@ -3077,7 +3095,7 @@
       <c r="D32" s="61"/>
       <c r="E32" s="62">
         <f>SUM(E9:E31)</f>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F32" s="63"/>
       <c r="G32" s="64" t="s">
@@ -3094,7 +3112,7 @@
       </c>
       <c r="O32" s="68">
         <f>SUM(O9:O31)</f>
-        <v>5</v>
+        <v>140.49</v>
       </c>
       <c r="P32" s="47"/>
       <c r="Q32" s="19"/>
@@ -3122,15 +3140,15 @@
       <c r="A34" s="27"/>
       <c r="B34" s="70"/>
       <c r="C34" s="70"/>
-      <c r="D34" s="76"/>
-      <c r="E34" s="76"/>
-      <c r="F34" s="76"/>
-      <c r="G34" s="76"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
-      <c r="K34" s="76"/>
-      <c r="L34" s="76"/>
+      <c r="D34" s="78"/>
+      <c r="E34" s="78"/>
+      <c r="F34" s="78"/>
+      <c r="G34" s="78"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="78"/>
+      <c r="J34" s="78"/>
+      <c r="K34" s="78"/>
+      <c r="L34" s="78"/>
       <c r="M34" s="70"/>
       <c r="N34" s="70"/>
       <c r="O34" s="70"/>
@@ -3141,15 +3159,15 @@
       <c r="A35" s="27"/>
       <c r="B35" s="70"/>
       <c r="C35" s="70"/>
-      <c r="D35" s="76"/>
-      <c r="E35" s="76"/>
-      <c r="F35" s="76"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
+      <c r="D35" s="78"/>
+      <c r="E35" s="78"/>
+      <c r="F35" s="78"/>
+      <c r="G35" s="78"/>
+      <c r="H35" s="78"/>
+      <c r="I35" s="78"/>
+      <c r="J35" s="78"/>
+      <c r="K35" s="78"/>
+      <c r="L35" s="78"/>
       <c r="M35" s="70"/>
       <c r="N35" s="70"/>
       <c r="O35" s="70"/>
@@ -3160,15 +3178,15 @@
       <c r="A36" s="71"/>
       <c r="B36" s="72"/>
       <c r="C36" s="72"/>
-      <c r="D36" s="77"/>
-      <c r="E36" s="77"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="77"/>
-      <c r="K36" s="77"/>
-      <c r="L36" s="77"/>
+      <c r="D36" s="79"/>
+      <c r="E36" s="79"/>
+      <c r="F36" s="79"/>
+      <c r="G36" s="79"/>
+      <c r="H36" s="79"/>
+      <c r="I36" s="79"/>
+      <c r="J36" s="79"/>
+      <c r="K36" s="79"/>
+      <c r="L36" s="79"/>
       <c r="M36" s="72"/>
       <c r="N36" s="72"/>
       <c r="O36" s="72"/>

</xml_diff>